<commit_message>
minor adjustment on import excel
</commit_message>
<xml_diff>
--- a/Format.xlsx
+++ b/Format.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\reportIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E469D84-3432-4545-BC13-1075305B9B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="208"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>No</t>
   </si>
@@ -88,13 +89,121 @@
   </si>
   <si>
     <t>Spesifikasi</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>Komputer</t>
+  </si>
+  <si>
+    <t>Handphone</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>Kamera</t>
+  </si>
+  <si>
+    <t>Mouse</t>
+  </si>
+  <si>
+    <t>Parabola</t>
+  </si>
+  <si>
+    <t>Kabel</t>
+  </si>
+  <si>
+    <t>Status Kebutuhan</t>
+  </si>
+  <si>
+    <t>Pergantian Barang</t>
+  </si>
+  <si>
+    <t>Perbaikan Barang</t>
+  </si>
+  <si>
+    <t>Kerusakan Barang</t>
+  </si>
+  <si>
+    <t>Permintaan Barang</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Board Of Director</t>
+  </si>
+  <si>
+    <t>Billing Support</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Finance &amp; Accounting</t>
+  </si>
+  <si>
+    <t>Human Resource</t>
+  </si>
+  <si>
+    <t>HUB Operation</t>
+  </si>
+  <si>
+    <t>Legal</t>
+  </si>
+  <si>
+    <t>MP Upgrade</t>
+  </si>
+  <si>
+    <t>General Affair</t>
+  </si>
+  <si>
+    <t>Services Delivery</t>
+  </si>
+  <si>
+    <t>Product Development</t>
+  </si>
+  <si>
+    <t>Purchasing</t>
+  </si>
+  <si>
+    <t>QMR</t>
+  </si>
+  <si>
+    <t>Sales &amp; Marketing</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Warehouse &amp; Logistic</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>Business Support</t>
+  </si>
+  <si>
+    <t>NIX</t>
+  </si>
+  <si>
+    <t>Bitnet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -107,6 +216,18 @@
       <family val="2"/>
       <charset val="1"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF444444"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -190,7 +311,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -210,10 +331,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -505,10 +628,15 @@
     <col min="4" max="4" width="19.6640625"/>
     <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="1025" width="11.5546875"/>
+    <col min="7" max="8" width="11.5546875"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="25" width="11.5546875"/>
+    <col min="26" max="26" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="1025" width="11.5546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="58.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -578,10 +706,172 @@
       <c r="W1" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="Z1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="Z11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="28:28" x14ac:dyDescent="0.25">
+      <c r="AB21" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{94B9C62C-E3E1-4B79-9773-77D39D812030}">
+      <formula1>$Z$2:$Z$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{0C63999A-FD33-41EE-89C0-363CB69DB9F9}">
+      <formula1>$AA$2:$AA$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{898AB907-A28F-4F95-B07A-1DEF0D19198D}">
+      <formula1>$AB$2:$AB$21</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>